<commit_message>
made changes to possibility filter
</commit_message>
<xml_diff>
--- a/Downloads/Possibility Filter V6.xlsx
+++ b/Downloads/Possibility Filter V6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\hipoha-framework\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF87127-8646-4FE9-B6C4-BAD3176EA076}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C4DC97-017B-4C0C-BB7C-6DA85F046417}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B3A634E3-7B0D-49A1-AC45-20D6757FFE73}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>ID</t>
   </si>
@@ -120,9 +120,6 @@
   </si>
   <si>
     <t>TRAFFIC LIGHT MODEL</t>
-  </si>
-  <si>
-    <t>not tested</t>
   </si>
   <si>
     <t>P13</t>
@@ -228,28 +225,25 @@
     </r>
   </si>
   <si>
-    <t>Customer Support executive</t>
-  </si>
-  <si>
     <t>Fast &amp; Economic</t>
   </si>
   <si>
-    <t>Have a separate phone for sending this whatsapp</t>
-  </si>
-  <si>
-    <t>Sending "How-To" video by whatsapp to new customer based on excel data</t>
-  </si>
-  <si>
-    <t>RPA to read excel and then post into Whatsapp</t>
-  </si>
-  <si>
-    <t>Have another executice handle this step</t>
-  </si>
-  <si>
-    <t>No expertise on RPA</t>
-  </si>
-  <si>
-    <t>Make an function in excel to create hyperlink to post to web whatsapp</t>
+    <t>Identify which mentee or squad needs mentoring</t>
+  </si>
+  <si>
+    <t>Mentor</t>
+  </si>
+  <si>
+    <t>Make a report with Power BI</t>
+  </si>
+  <si>
+    <t>No expertise in Power BI</t>
+  </si>
+  <si>
+    <t>Make a report screen with Vue.js + microservices</t>
+  </si>
+  <si>
+    <t>Need to develop APIs &amp; Slice &amp; Dice front end screen</t>
   </si>
 </sst>
 </file>
@@ -1437,8 +1431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F2573A-FEAE-4632-8EED-3B01D309CD71}">
   <dimension ref="B1:AB42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:G10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16:E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,7 +1453,7 @@
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="47" t="s">
@@ -1520,17 +1514,17 @@
     <row r="7" spans="2:9" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="12"/>
       <c r="C7" s="43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I7" s="11"/>
     </row>
     <row r="8" spans="2:9" s="20" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="17"/>
       <c r="C8" s="42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" s="53" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E8" s="54"/>
       <c r="F8" s="54"/>
@@ -1541,10 +1535,10 @@
     <row r="9" spans="2:9" s="20" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="17"/>
       <c r="C9" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9" s="50" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E9" s="51"/>
       <c r="F9" s="51"/>
@@ -1555,10 +1549,10 @@
     <row r="10" spans="2:9" s="20" customFormat="1" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="17"/>
       <c r="C10" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="50" t="s">
         <v>43</v>
-      </c>
-      <c r="D10" s="50" t="s">
-        <v>45</v>
       </c>
       <c r="E10" s="51"/>
       <c r="F10" s="51"/>
@@ -1601,57 +1595,57 @@
         <v>2</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D13" s="33">
         <v>1</v>
       </c>
       <c r="E13" s="33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13" s="28">
         <f>AVERAGE('Listing out possibilities'!$D13:$E13)</f>
-        <v>1</v>
-      </c>
-      <c r="G13" s="36"/>
+        <v>1.5</v>
+      </c>
+      <c r="G13" s="36" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D14" s="39">
         <v>1</v>
       </c>
       <c r="E14" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" s="29">
         <f>AVERAGE('Listing out possibilities'!$D14:$E14)</f>
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="G14" s="37" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="32" t="s">
-        <v>49</v>
-      </c>
+      <c r="C15" s="32"/>
       <c r="D15" s="33">
         <v>1</v>
       </c>
       <c r="E15" s="33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F15" s="28">
         <f>AVERAGE('Listing out possibilities'!$D15:$E15)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G15" s="36"/>
     </row>
@@ -1659,9 +1653,7 @@
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="32" t="s">
-        <v>51</v>
-      </c>
+      <c r="C16" s="32"/>
       <c r="D16" s="39">
         <v>3</v>
       </c>
@@ -1679,10 +1671,10 @@
         <v>6</v>
       </c>
       <c r="C17" s="32"/>
-      <c r="D17" s="33">
-        <v>3</v>
-      </c>
-      <c r="E17" s="33">
+      <c r="D17" s="39">
+        <v>3</v>
+      </c>
+      <c r="E17" s="39">
         <v>3</v>
       </c>
       <c r="F17" s="28">
@@ -1713,15 +1705,15 @@
         <v>10</v>
       </c>
       <c r="C19" s="32"/>
-      <c r="D19" s="33">
-        <v>2</v>
-      </c>
-      <c r="E19" s="33">
-        <v>2</v>
+      <c r="D19" s="39">
+        <v>3</v>
+      </c>
+      <c r="E19" s="39">
+        <v>3</v>
       </c>
       <c r="F19" s="28">
         <f>AVERAGE('Listing out possibilities'!$D19:$E19)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G19" s="36"/>
     </row>
@@ -1747,15 +1739,15 @@
         <v>14</v>
       </c>
       <c r="C21" s="32"/>
-      <c r="D21" s="33">
-        <v>1</v>
-      </c>
-      <c r="E21" s="33">
-        <v>1</v>
+      <c r="D21" s="39">
+        <v>3</v>
+      </c>
+      <c r="E21" s="39">
+        <v>3</v>
       </c>
       <c r="F21" s="28">
         <f>AVERAGE('Listing out possibilities'!$D21:$E21)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G21" s="36"/>
       <c r="AB21" s="2">
@@ -1777,9 +1769,7 @@
         <f>AVERAGE('Listing out possibilities'!$D22:$E22)</f>
         <v>3</v>
       </c>
-      <c r="G22" s="37" t="s">
-        <v>20</v>
-      </c>
+      <c r="G22" s="37"/>
       <c r="AB22" s="2">
         <v>2</v>
       </c>
@@ -1789,10 +1779,10 @@
         <v>16</v>
       </c>
       <c r="C23" s="32"/>
-      <c r="D23" s="33">
-        <v>3</v>
-      </c>
-      <c r="E23" s="33">
+      <c r="D23" s="39">
+        <v>3</v>
+      </c>
+      <c r="E23" s="39">
         <v>3</v>
       </c>
       <c r="F23" s="28">
@@ -1813,23 +1803,23 @@
         <v>3</v>
       </c>
       <c r="E24" s="39">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F24" s="29">
         <f>AVERAGE('Listing out possibilities'!$D24:$E24)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G24" s="37"/>
     </row>
     <row r="25" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C25" s="32"/>
-      <c r="D25" s="33">
-        <v>3</v>
-      </c>
-      <c r="E25" s="33">
+      <c r="D25" s="39">
+        <v>3</v>
+      </c>
+      <c r="E25" s="39">
         <v>3</v>
       </c>
       <c r="F25" s="28">
@@ -1840,7 +1830,7 @@
     </row>
     <row r="26" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C26" s="34"/>
       <c r="D26" s="39">
@@ -1857,13 +1847,13 @@
     </row>
     <row r="27" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C27" s="32"/>
-      <c r="D27" s="33">
-        <v>3</v>
-      </c>
-      <c r="E27" s="33">
+      <c r="D27" s="39">
+        <v>3</v>
+      </c>
+      <c r="E27" s="39">
         <v>3</v>
       </c>
       <c r="F27" s="28">
@@ -1874,7 +1864,7 @@
     </row>
     <row r="28" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C28" s="34"/>
       <c r="D28" s="39">
@@ -1891,13 +1881,13 @@
     </row>
     <row r="29" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C29" s="32"/>
-      <c r="D29" s="33">
-        <v>3</v>
-      </c>
-      <c r="E29" s="33">
+      <c r="D29" s="39">
+        <v>3</v>
+      </c>
+      <c r="E29" s="39">
         <v>3</v>
       </c>
       <c r="F29" s="28">
@@ -1908,7 +1898,7 @@
     </row>
     <row r="30" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C30" s="34"/>
       <c r="D30" s="39">
@@ -1925,13 +1915,13 @@
     </row>
     <row r="31" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C31" s="34"/>
-      <c r="D31" s="33">
-        <v>3</v>
-      </c>
-      <c r="E31" s="33">
+      <c r="D31" s="39">
+        <v>3</v>
+      </c>
+      <c r="E31" s="39">
         <v>3</v>
       </c>
       <c r="F31" s="28">
@@ -1942,7 +1932,7 @@
     </row>
     <row r="32" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C32" s="34"/>
       <c r="D32" s="39">
@@ -1959,13 +1949,13 @@
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C33" s="34"/>
-      <c r="D33" s="33">
-        <v>3</v>
-      </c>
-      <c r="E33" s="33">
+      <c r="D33" s="39">
+        <v>3</v>
+      </c>
+      <c r="E33" s="39">
         <v>3</v>
       </c>
       <c r="F33" s="28">
@@ -1976,7 +1966,7 @@
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C34" s="34"/>
       <c r="D34" s="39">
@@ -1993,7 +1983,7 @@
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C35" s="34"/>
       <c r="D35" s="39">
@@ -2010,7 +2000,7 @@
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C36" s="34"/>
       <c r="D36" s="39">
@@ -2027,13 +2017,13 @@
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C37" s="34"/>
-      <c r="D37" s="33">
-        <v>3</v>
-      </c>
-      <c r="E37" s="33">
+      <c r="D37" s="39">
+        <v>3</v>
+      </c>
+      <c r="E37" s="39">
         <v>3</v>
       </c>
       <c r="F37" s="28">
@@ -2046,7 +2036,7 @@
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C38" s="34"/>
       <c r="D38" s="39">
@@ -2063,7 +2053,7 @@
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C39" s="34"/>
       <c r="D39" s="39">
@@ -2080,7 +2070,7 @@
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C40" s="34"/>
       <c r="D40" s="39">
@@ -2097,7 +2087,7 @@
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C41" s="34"/>
       <c r="D41" s="33">
@@ -2114,7 +2104,7 @@
     </row>
     <row r="42" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C42" s="35"/>
       <c r="D42" s="40">

</xml_diff>

<commit_message>
Update Possibility Filter V6.xlsx
</commit_message>
<xml_diff>
--- a/Downloads/Possibility Filter V6.xlsx
+++ b/Downloads/Possibility Filter V6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\hipoha-framework\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C4DC97-017B-4C0C-BB7C-6DA85F046417}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F8A1FA-2A05-4DEB-9391-DCE1C4F61585}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B3A634E3-7B0D-49A1-AC45-20D6757FFE73}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>ID</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>Need to develop APIs &amp; Slice &amp; Dice front end screen</t>
+  </si>
+  <si>
+    <t>Start excel</t>
   </si>
 </sst>
 </file>
@@ -1431,8 +1434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F2573A-FEAE-4632-8EED-3B01D309CD71}">
   <dimension ref="B1:AB42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16:E39"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1636,16 +1639,18 @@
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="32"/>
+      <c r="C15" s="32" t="s">
+        <v>50</v>
+      </c>
       <c r="D15" s="33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E15" s="33">
         <v>3</v>
       </c>
       <c r="F15" s="28">
         <f>AVERAGE('Listing out possibilities'!$D15:$E15)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G15" s="36"/>
     </row>

</xml_diff>